<commit_message>
Atualização do dia 03/05/2023
</commit_message>
<xml_diff>
--- a/documentação/Backlog_requisitos.xlsx
+++ b/documentação/Backlog_requisitos.xlsx
@@ -476,19 +476,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -808,7 +808,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,17 +845,17 @@
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
-      <c r="B5" s="30" t="s">
+      <c r="A5" s="27"/>
+      <c r="B5" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="27"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="30"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
     </row>
@@ -870,10 +870,10 @@
       <c r="D6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="26" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -958,7 +958,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>25</v>
@@ -1045,7 +1045,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>26</v>

</xml_diff>